<commit_message>
Updates to regex matching to make sure divs across multiple lines don't error
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-caculated-age.xlsx
+++ b/output/StructureDefinition-eicr-anon-caculated-age.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-28T20:58:40+10:00</t>
+    <t>2024-06-29T16:05:37+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -407,7 +407,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-eicr-anon-text:text.div SHALL be '&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;&lt;p&gt;MASKED&lt;/p&gt;&lt;/div&gt;' {`div` ~ '&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;&lt;p&gt;MASKED&lt;/p&gt;&lt;/div&gt;'}</t>
+eicr-anon-text:text.div SHALL be '&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;&lt;p&gt;MASKED&lt;/p&gt;&lt;/div&gt;' {exists() implies `div`.toString().matches('&lt;div xmlns="http://www.w3.org/1999/xhtml"&gt;\\s*&lt;p&gt;MASKED&lt;/p&gt;\\s*&lt;/div&gt;')}</t>
   </si>
   <si>
     <t>Act.text?</t>

</xml_diff>